<commit_message>
Raw data for PMID 27711131
</commit_message>
<xml_diff>
--- a/Datasets/27711131/raw_data/journal.pone.0164175.s006.xlsx
+++ b/Datasets/27711131/raw_data/journal.pone.0164175.s006.xlsx
@@ -2330,13 +2330,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C411B176-B2B3-8840-A538-082E74E9EF3C}" diskRevisions="1" revisionId="522" version="2">
-  <header guid="{51A3828C-9893-3447-B576-0EF38ECA5CF2}" dateTime="2016-08-02T12:08:42" maxSheetId="4" userName="Lubomir Tomaska" r:id="rId1" minRId="522">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
   <header guid="{B6290C78-16FD-484D-B34E-565A4C56B631}" dateTime="2016-08-02T15:19:36" maxSheetId="4" userName="Lubomir Tomaska" r:id="rId2">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -2354,53 +2347,6 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="522" sId="1">
-    <oc r="A1" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="14"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>S2 Table</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>. List of mutants exhibiting an altered sensitivity to valinomycin and/or nigericin</t>
-        </r>
-      </is>
-    </oc>
-    <nc r="A1" t="inlineStr">
-      <is>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="14"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>S3 Table</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>. List of mutants exhibiting an altered sensitivity to valinomycin and/or nigericin</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{0E92359C-4E55-6643-99C2-43983B6D4AE6}" action="delete"/>
@@ -2415,9 +2361,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
-  <userInfo guid="{B6290C78-16FD-484D-B34E-565A4C56B631}" name="Anastasia Baryshnikova" id="-348860353" dateTime="2016-10-19T13:47:23"/>
-</users>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>